<commit_message>
Added the remaining test cases
</commit_message>
<xml_diff>
--- a/Test Cases/Test Case 1/Input/Input.xlsx
+++ b/Test Cases/Test Case 1/Input/Input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Drilling Dynamics\Soft String Research Project\Model Evaluation\Drill String Test Cases\Test Cases\Test Case 1\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elmir.hamidov\Desktop\Workspace\Drill-String-Test-Cases\Test Cases\Test Case 1\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3F8943-9555-444F-A701-DEE3BB0E7241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA03DF74-5569-4101-AA91-525A876DFCEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46470" yWindow="-1755" windowWidth="19020" windowHeight="15885" xr2:uid="{BBAEC26E-AC9D-4421-A399-37DF8CFE6789}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{BBAEC26E-AC9D-4421-A399-37DF8CFE6789}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Parameter</t>
   </si>
@@ -57,20 +57,83 @@
     <t xml:space="preserve">ρ </t>
   </si>
   <si>
-    <t>lb/f t</t>
-  </si>
-  <si>
     <t xml:space="preserve">kg/m3 </t>
   </si>
   <si>
     <t>Drill pipe density</t>
+  </si>
+  <si>
+    <t>G_DP</t>
+  </si>
+  <si>
+    <t>OD_DP</t>
+  </si>
+  <si>
+    <t>ID_DP</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Shear modulus</t>
+  </si>
+  <si>
+    <t>Drill pipe outer diameter</t>
+  </si>
+  <si>
+    <t>Drill pipe inner diameter</t>
+  </si>
+  <si>
+    <t>Bit depth</t>
+  </si>
+  <si>
+    <t>Measured depth</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>lbf/ft2</t>
+  </si>
+  <si>
+    <t>lb/ft3</t>
+  </si>
+  <si>
+    <t>f_s</t>
+  </si>
+  <si>
+    <t>f_d</t>
+  </si>
+  <si>
+    <t>Static friction factor</t>
+  </si>
+  <si>
+    <t>Dynamic friction factor</t>
+  </si>
+  <si>
+    <t>MD [m]</t>
+  </si>
+  <si>
+    <t>INC [°]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +149,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -95,7 +165,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -113,17 +183,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -133,15 +192,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -478,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2665F497-93D1-4D8F-B473-96F38BF40306}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+      <selection activeCell="C17" sqref="C16:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,37 +568,167 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>490.6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2">
+        <v>7850</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>7850</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="B3" s="3">
+        <f>1670000000</f>
+        <v>1670000000</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="3">
+        <f>79900000000</f>
+        <v>79900000000</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5.88</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.127</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5905.5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1800</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6561.7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -540,12 +738,296 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34730D62-7317-40D9-8831-9111EE2571B8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <f>A2+100</f>
+        <v>100</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <f t="shared" ref="A4:A42" si="0">A3+100</f>
+        <v>200</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="B6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="B15" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="B16" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>1600</v>
+      </c>
+      <c r="B18" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+      <c r="B19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+      <c r="B20" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <f t="shared" si="0"/>
+        <v>1900</v>
+      </c>
+      <c r="B21" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="B22" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>